<commit_message>
Updated analysis code ad figures
</commit_message>
<xml_diff>
--- a/RSVP_visual_now/Results/RSVP_spatial_cue_ISI_presentation/RSVP_spatial_cue_ISI_presentationsubject_level_stats.xlsx
+++ b/RSVP_visual_now/Results/RSVP_spatial_cue_ISI_presentation/RSVP_spatial_cue_ISI_presentationsubject_level_stats.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -785,6 +785,110 @@
         <v>0.01769911504424779</v>
       </c>
     </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-0.22</v>
+      </c>
+      <c r="F16" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-0.08620689655172414</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.008474576271186441</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="D17" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-0.24</v>
+      </c>
+      <c r="F17" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="G17" t="n">
+        <v>-0.1185185185185185</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.1467889908256881</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>17</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-0.14</v>
+      </c>
+      <c r="F18" t="n">
+        <v>2.49</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-0.1129032258064516</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>18</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="G19" t="n">
+        <v>-0.140625</v>
+      </c>
+      <c r="H19" t="n">
+        <v>-0.1810344827586207</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>